<commit_message>
2016-07-26  Create Slide Proxy
</commit_message>
<xml_diff>
--- a/Document/BangPhanCong.xlsx
+++ b/Document/BangPhanCong.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khoa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebForm\GNSeaCorp\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -107,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,7 +408,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,6 +497,9 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
+      <c r="F5" s="1">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -523,6 +527,9 @@
       </c>
       <c r="E7" t="s">
         <v>13</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>